<commit_message>
Full resnet-50 graph is completed for both inference and BP.
</commit_message>
<xml_diff>
--- a/ColtrainISA.xlsx
+++ b/ColtrainISA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t xml:space="preserve">opcode</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">MULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULT_DER</t>
   </si>
   <si>
     <t xml:space="preserve">ADD</t>
@@ -211,17 +214,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.43"/>
   </cols>
@@ -322,7 +325,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -333,7 +336,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -344,41 +347,38 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,27 +386,27 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,12 +419,26 @@
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Both FW and BP for both resnet50 and lstm is done.
</commit_message>
<xml_diff>
--- a/ColtrainISA.xlsx
+++ b/ColtrainISA.xlsx
@@ -217,7 +217,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -225,7 +225,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.43"/>
   </cols>
   <sheetData>

</xml_diff>